<commit_message>
Updated notebooks and readme file
</commit_message>
<xml_diff>
--- a/Data/Airline_balsheet.xlsx
+++ b/Data/Airline_balsheet.xlsx
@@ -39,9 +39,6 @@
     <t>Total Current Assets</t>
   </si>
   <si>
-    <t>Other Long-Term Assets</t>
-  </si>
-  <si>
     <t>Total Assets</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>Long Term Debt</t>
+  </si>
+  <si>
+    <t>Other Long Term Assets</t>
   </si>
 </sst>
 </file>
@@ -520,22 +520,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.83203125" customWidth="1"/>
     <col min="13" max="13" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.33203125" bestFit="1" customWidth="1"/>
@@ -562,60 +562,60 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2">
         <v>44285</v>
@@ -624,7 +624,7 @@
         <v>2021</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
         <v>44300</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>44195</v>
@@ -692,7 +692,7 @@
         <v>2020</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
         <v>44209</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2">
         <v>44103</v>
@@ -760,7 +760,7 @@
         <v>2020</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2">
         <v>44122</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
         <v>44011</v>
@@ -828,7 +828,7 @@
         <v>2020</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2">
         <v>44026</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2">
         <v>44285</v>
@@ -896,7 +896,7 @@
         <v>2021</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2">
         <v>44307</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2">
         <v>44195</v>
@@ -964,7 +964,7 @@
         <v>2020</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2">
         <v>44223</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>44103</v>
@@ -1032,7 +1032,7 @@
         <v>2020</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="2">
         <v>44126</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2">
         <v>44011</v>
@@ -1100,7 +1100,7 @@
         <v>2020</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="2">
         <v>44035</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2">
         <v>44285</v>
@@ -1168,7 +1168,7 @@
         <v>2021</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2">
         <v>44305</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2">
         <v>44195</v>
@@ -1236,7 +1236,7 @@
         <v>2020</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2">
         <v>44216</v>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2">
         <v>44103</v>
@@ -1304,7 +1304,7 @@
         <v>2020</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="2">
         <v>44118</v>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
         <v>44011</v>
@@ -1372,7 +1372,7 @@
         <v>2020</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="2">
         <v>44033</v>

</xml_diff>